<commit_message>
Added a new section
</commit_message>
<xml_diff>
--- a/Table1.xlsx
+++ b/Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravichandrans\Documents\GitHub\ML-predict-drugclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5270CB21-DA77-401E-940C-133B114A20DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B564BE85-EFD6-4BD1-9E53-28E7EFBD467E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
   <si>
     <t>SMILES</t>
   </si>
@@ -43,24 +43,6 @@
     <t>SMILES1</t>
   </si>
   <si>
-    <t>FP1</t>
-  </si>
-  <si>
-    <t>FP2</t>
-  </si>
-  <si>
-    <t>FP3</t>
-  </si>
-  <si>
-    <t>FP4</t>
-  </si>
-  <si>
-    <t>FP5</t>
-  </si>
-  <si>
-    <t>FP6</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -119,12 +101,36 @@
   </si>
   <si>
     <t xml:space="preserve">Accuracy = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA = </t>
+  </si>
+  <si>
+    <t>sFP1</t>
+  </si>
+  <si>
+    <t>sFP2</t>
+  </si>
+  <si>
+    <t>sFP3</t>
+  </si>
+  <si>
+    <t>sFP4</t>
+  </si>
+  <si>
+    <t>sFP5</t>
+  </si>
+  <si>
+    <t>sFP6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,14 +420,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,15 +712,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q24:Q25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26:R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -722,25 +732,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -769,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -777,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -798,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -806,7 +816,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -827,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -835,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -856,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -864,7 +874,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -885,65 +895,349 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N27" s="1">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N28" s="1">
+        <v>2</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N29" s="1">
+        <v>3</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N30" s="1">
+        <v>3</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P30" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N31" s="1">
+        <v>4</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -956,30 +1250,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5CED93-420D-42A7-825A-02AD102038B3}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E19:F20"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="19" style="4"/>
+    <col min="1" max="1" width="19" style="4"/>
+    <col min="2" max="2" width="16.140625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="19" style="4"/>
+    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="19" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:5" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" s="10">
         <v>1</v>
@@ -994,7 +1292,7 @@
     </row>
     <row r="4" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="12">
         <v>1</v>
@@ -1017,14 +1315,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B7" s="19">
         <f xml:space="preserve"> (4/6)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" s="17">
         <f xml:space="preserve"> C3/C5</f>
@@ -1033,7 +1331,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C8" s="16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" s="18">
         <f xml:space="preserve">  D4/D5</f>
@@ -1042,7 +1340,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C9" s="16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9" s="17">
         <f xml:space="preserve"> (D7+D8)/2</f>
@@ -1052,18 +1350,18 @@
     <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:5" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C14" s="20">
         <v>890</v>
@@ -1078,7 +1376,7 @@
     </row>
     <row r="15" spans="1:5" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C15" s="12">
         <v>90</v>
@@ -1103,14 +1401,14 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="26">
+        <v>22</v>
+      </c>
+      <c r="B18" s="24">
         <f xml:space="preserve"> ( C14 + D15)/(E14 + E15)</f>
         <v>0.9</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D18" s="24">
         <f xml:space="preserve"> C14/C16</f>
@@ -1119,7 +1417,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C19" s="23" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D19" s="25">
         <f xml:space="preserve">  D15/D16</f>
@@ -1128,7 +1426,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C20" s="23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D20" s="24">
         <f xml:space="preserve"> (D18+D19)/2</f>

</xml_diff>